<commit_message>
added a 3rd trial and plotted averaged data on graphs
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>Number of nodes (N)</t>
   </si>
@@ -38,12 +38,24 @@
   <si>
     <t>Delay_1</t>
   </si>
+  <si>
+    <t>Throughput_3</t>
+  </si>
+  <si>
+    <t>Delay_3</t>
+  </si>
+  <si>
+    <t>Average_TP</t>
+  </si>
+  <si>
+    <t>Average_Delay</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -67,8 +79,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -84,6 +104,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -106,7 +132,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -118,24 +144,43 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -222,24 +267,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$6</c:f>
+              <c:f>Sheet1!$I$2:$I$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>22.8</c:v>
+                  <c:v>23.64</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45.48</c:v>
+                  <c:v>45.88</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>69.48</c:v>
+                  <c:v>69.44</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>93.72</c:v>
+                  <c:v>91.72000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>117.24</c:v>
+                  <c:v>115.48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -281,24 +326,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$7:$C$11</c:f>
+              <c:f>Sheet1!$I$7:$I$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>33.36</c:v>
+                  <c:v>30.04</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55.8</c:v>
+                  <c:v>56.52</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>80.28</c:v>
+                  <c:v>82.96</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>113.04</c:v>
+                  <c:v>109.76</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>132.36</c:v>
+                  <c:v>134.32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -340,24 +385,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$12:$C$16</c:f>
+              <c:f>Sheet1!$I$12:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>30.84</c:v>
+                  <c:v>33.08000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64.32</c:v>
+                  <c:v>65.52</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>96.96</c:v>
+                  <c:v>97.24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128.88</c:v>
+                  <c:v>126.64</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>154.56</c:v>
+                  <c:v>156.48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -374,11 +419,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="364455608"/>
-        <c:axId val="364457016"/>
+        <c:axId val="2073204840"/>
+        <c:axId val="2073198040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="364455608"/>
+        <c:axId val="2073204840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -407,7 +452,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="364457016"/>
+        <c:crossAx val="2073198040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -415,7 +460,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="364457016"/>
+        <c:axId val="2073198040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -445,7 +490,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="364455608"/>
+        <c:crossAx val="2073204840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -546,24 +591,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$6</c:f>
+              <c:f>Sheet1!$J$2:$J$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>460235.552632</c:v>
+                  <c:v>457044.330189</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>464609.883905</c:v>
+                  <c:v>466580.4422046666</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>468212.708117</c:v>
+                  <c:v>462241.132387</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>472881.133163</c:v>
+                  <c:v>470272.919111</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>459679.492323</c:v>
+                  <c:v>470644.8508590001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -605,24 +650,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$7:$E$11</c:f>
+              <c:f>Sheet1!$J$7:$J$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>468461.266187</c:v>
+                  <c:v>473072.300318</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>470468.705376</c:v>
+                  <c:v>472931.2569146667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>485059.892377</c:v>
+                  <c:v>480578.8520713334</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>470073.940552</c:v>
+                  <c:v>469887.9772243334</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>471441.261106</c:v>
+                  <c:v>475591.5233153333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -664,24 +709,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$12:$E$16</c:f>
+              <c:f>Sheet1!$J$12:$J$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>451218.626459</c:v>
+                  <c:v>461123.9219793333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>475690.669776</c:v>
+                  <c:v>478432.755821</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>487431.055693</c:v>
+                  <c:v>480536.6169313334</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>474182.888268</c:v>
+                  <c:v>477101.0885969999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>484451.771739</c:v>
+                  <c:v>479913.171336</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -698,11 +743,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="485230152"/>
-        <c:axId val="424618296"/>
+        <c:axId val="2073127848"/>
+        <c:axId val="2073122312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="485230152"/>
+        <c:axId val="2073127848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -731,7 +776,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="424618296"/>
+        <c:crossAx val="2073122312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -739,7 +784,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="424618296"/>
+        <c:axId val="2073122312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -769,7 +814,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="485230152"/>
+        <c:crossAx val="2073127848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -870,24 +915,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$23</c:f>
+              <c:f>Sheet1!$I$19:$I$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>18.12</c:v>
+                  <c:v>19.64</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.72</c:v>
+                  <c:v>36.36</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60.12</c:v>
+                  <c:v>57.32</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75.12</c:v>
+                  <c:v>74.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>89.16</c:v>
+                  <c:v>89.56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -929,24 +974,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$24:$C$28</c:f>
+              <c:f>Sheet1!$I$24:$I$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>27.96</c:v>
+                  <c:v>28.56</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55.2</c:v>
+                  <c:v>56.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>81.12</c:v>
+                  <c:v>81.44</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>110.88</c:v>
+                  <c:v>111.48</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>138.12</c:v>
+                  <c:v>136.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -988,24 +1033,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$29:$C$33</c:f>
+              <c:f>Sheet1!$I$29:$I$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>39.72</c:v>
+                  <c:v>37.56</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>73.32</c:v>
+                  <c:v>74.52</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110.88</c:v>
+                  <c:v>112.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>141.6</c:v>
+                  <c:v>142.88</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>170.16</c:v>
+                  <c:v>173.92</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1022,11 +1067,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="487250536"/>
-        <c:axId val="486170344"/>
+        <c:axId val="2073086456"/>
+        <c:axId val="2073080680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="487250536"/>
+        <c:axId val="2073086456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1060,7 +1105,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="486170344"/>
+        <c:crossAx val="2073080680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1068,7 +1113,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="486170344"/>
+        <c:axId val="2073080680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1098,7 +1143,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="487250536"/>
+        <c:crossAx val="2073086456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1194,24 +1239,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$19:$E$23</c:f>
+              <c:f>Sheet1!$J$19:$J$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>468820.264901</c:v>
+                  <c:v>459241.8765253333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>501809.343137</c:v>
+                  <c:v>479207.6873823334</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>485758.556886</c:v>
+                  <c:v>484477.2630726666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>489340.889776</c:v>
+                  <c:v>490616.687429</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>498481.483176</c:v>
+                  <c:v>491929.249841</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1253,24 +1298,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$24:$E$28</c:f>
+              <c:f>Sheet1!$J$24:$J$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>444805.042918</c:v>
+                  <c:v>455371.7438486666</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>489640.41087</c:v>
+                  <c:v>482930.413455</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>490069.198225</c:v>
+                  <c:v>487542.9302906667</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>487602.008658</c:v>
+                  <c:v>493282.007499</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>508393.59861</c:v>
+                  <c:v>499561.836133</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1312,24 +1357,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$29:$E$33</c:f>
+              <c:f>Sheet1!$J$29:$J$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>464118.033233</c:v>
+                  <c:v>460283.83121</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>477664.090016</c:v>
+                  <c:v>480831.7651826666</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>497298.042208</c:v>
+                  <c:v>490162.188937</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>495738.574576</c:v>
+                  <c:v>491219.783169</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>494869.557828</c:v>
+                  <c:v>498669.63218</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1346,11 +1391,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="487561832"/>
-        <c:axId val="486496088"/>
+        <c:axId val="2073045704"/>
+        <c:axId val="2073040168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="487561832"/>
+        <c:axId val="2073045704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1379,7 +1424,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="486496088"/>
+        <c:crossAx val="2073040168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1387,7 +1432,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="486496088"/>
+        <c:axId val="2073040168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1417,7 +1462,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="487561832"/>
+        <c:crossAx val="2073045704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1443,16 +1488,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>507999</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>188118</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>530411</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>188865</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>126999</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>73818</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>274169</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>78300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1473,16 +1518,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>222250</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>69056</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>736973</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>30956</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>145256</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>355973</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>107156</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1503,16 +1548,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>396874</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>556745</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>140494</xdr:rowOff>
+      <xdr:rowOff>49353</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>15874</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>26194</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>304239</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>125553</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1533,16 +1578,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>238124</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>610159</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>148431</xdr:rowOff>
+      <xdr:rowOff>56543</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>682624</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>34131</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>232894</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>136478</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1886,10 +1931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G10" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="T22" sqref="T22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1897,9 +1942,12 @@
     <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1918,8 +1966,20 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>5</v>
       </c>
@@ -1938,8 +1998,22 @@
       <c r="F2" s="2">
         <v>459424.02500000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="2">
+        <v>24.12</v>
+      </c>
+      <c r="H2" s="2">
+        <v>451473.41293499997</v>
+      </c>
+      <c r="I2" s="5">
+        <f>AVERAGE(C2,D2,G2)</f>
+        <v>23.64</v>
+      </c>
+      <c r="J2" s="5">
+        <f>AVERAGE(E2,F2,H2)</f>
+        <v>457044.33018899994</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="B3">
         <v>40</v>
       </c>
@@ -1955,8 +2029,22 @@
       <c r="F3">
         <v>459099.710938</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <v>46.08</v>
+      </c>
+      <c r="H3">
+        <v>476031.73177100002</v>
+      </c>
+      <c r="I3" s="4">
+        <f t="shared" ref="I3:I16" si="0">AVERAGE(C3,D3,G3)</f>
+        <v>45.879999999999995</v>
+      </c>
+      <c r="J3" s="4">
+        <f t="shared" ref="J3:J16" si="1">AVERAGE(E3,F3,H3)</f>
+        <v>466580.44220466661</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="B4">
         <v>60</v>
       </c>
@@ -1972,8 +2060,22 @@
       <c r="F4">
         <v>463671.60512800002</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>68.64</v>
+      </c>
+      <c r="H4">
+        <v>454839.08391599997</v>
+      </c>
+      <c r="I4" s="4">
+        <f t="shared" si="0"/>
+        <v>69.44</v>
+      </c>
+      <c r="J4" s="4">
+        <f t="shared" si="1"/>
+        <v>462241.13238699996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="B5">
         <v>80</v>
       </c>
@@ -1989,8 +2091,22 @@
       <c r="F5">
         <v>470111.44502599997</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <v>89.76</v>
+      </c>
+      <c r="H5">
+        <v>467826.17914399999</v>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" si="0"/>
+        <v>91.720000000000013</v>
+      </c>
+      <c r="J5" s="4">
+        <f t="shared" si="1"/>
+        <v>470272.91911099997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="B6">
         <v>100</v>
       </c>
@@ -2006,8 +2122,22 @@
       <c r="F6">
         <v>478877.22292299999</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <v>115.08</v>
+      </c>
+      <c r="H6">
+        <v>473377.83733100002</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" si="0"/>
+        <v>115.48</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" si="1"/>
+        <v>470644.85085900006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2026,8 +2156,22 @@
       <c r="F7" s="2">
         <v>470033.29288700002</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="2">
+        <v>28.08</v>
+      </c>
+      <c r="H7" s="2">
+        <v>480722.34188000002</v>
+      </c>
+      <c r="I7" s="5">
+        <f t="shared" si="0"/>
+        <v>30.040000000000003</v>
+      </c>
+      <c r="J7" s="5">
+        <f t="shared" si="1"/>
+        <v>473072.30031799997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="B8">
         <v>40</v>
       </c>
@@ -2043,8 +2187,22 @@
       <c r="F8">
         <v>477924.73347099999</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <v>55.68</v>
+      </c>
+      <c r="H8">
+        <v>470400.33189700003</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="0"/>
+        <v>56.52</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" si="1"/>
+        <v>472931.25691466668</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="B9">
         <v>60</v>
       </c>
@@ -2060,8 +2218,22 @@
       <c r="F9">
         <v>473310.24225399998</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <v>83.4</v>
+      </c>
+      <c r="H9">
+        <v>483366.42158299999</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" si="0"/>
+        <v>82.960000000000008</v>
+      </c>
+      <c r="J9" s="4">
+        <f t="shared" si="1"/>
+        <v>480578.85207133339</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="B10">
         <v>80</v>
       </c>
@@ -2077,8 +2249,22 @@
       <c r="F10">
         <v>472367.87458399998</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10">
+        <v>108.12</v>
+      </c>
+      <c r="H10">
+        <v>467222.11653699999</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" si="0"/>
+        <v>109.76</v>
+      </c>
+      <c r="J10" s="4">
+        <f t="shared" si="1"/>
+        <v>469887.97722433339</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="B11">
         <v>100</v>
       </c>
@@ -2094,8 +2280,22 @@
       <c r="F11">
         <v>472948.32379200001</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11">
+        <v>136.44</v>
+      </c>
+      <c r="H11">
+        <v>482384.985048</v>
+      </c>
+      <c r="I11" s="4">
+        <f t="shared" si="0"/>
+        <v>134.32</v>
+      </c>
+      <c r="J11" s="4">
+        <f t="shared" si="1"/>
+        <v>475591.5233153333</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>7</v>
       </c>
@@ -2114,8 +2314,22 @@
       <c r="F12" s="2">
         <v>459703.19503499998</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" s="2">
+        <v>34.56</v>
+      </c>
+      <c r="H12" s="2">
+        <v>472449.94444400002</v>
+      </c>
+      <c r="I12" s="5">
+        <f t="shared" si="0"/>
+        <v>33.080000000000005</v>
+      </c>
+      <c r="J12" s="5">
+        <f t="shared" si="1"/>
+        <v>461123.92197933333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="B13">
         <v>40</v>
       </c>
@@ -2131,8 +2345,22 @@
       <c r="F13">
         <v>476965.169643</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13">
+        <v>65.040000000000006</v>
+      </c>
+      <c r="H13">
+        <v>482642.428044</v>
+      </c>
+      <c r="I13" s="4">
+        <f t="shared" si="0"/>
+        <v>65.52</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" si="1"/>
+        <v>478432.75582100003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="B14">
         <v>60</v>
       </c>
@@ -2148,8 +2376,22 @@
       <c r="F14">
         <v>479787.505428</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14">
+        <v>95.28</v>
+      </c>
+      <c r="H14">
+        <v>474391.28967299999</v>
+      </c>
+      <c r="I14" s="4">
+        <f t="shared" si="0"/>
+        <v>97.240000000000009</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" si="1"/>
+        <v>480536.61693133338</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="B15">
         <v>80</v>
       </c>
@@ -2165,8 +2407,22 @@
       <c r="F15">
         <v>481519.66091999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15">
+        <v>125.76</v>
+      </c>
+      <c r="H15">
+        <v>475600.71660300001</v>
+      </c>
+      <c r="I15" s="4">
+        <f t="shared" si="0"/>
+        <v>126.64</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" si="1"/>
+        <v>477101.08859699994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="B16">
         <v>100</v>
       </c>
@@ -2182,8 +2438,22 @@
       <c r="F16">
         <v>484112.718008</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G16">
+        <v>158.28</v>
+      </c>
+      <c r="H16">
+        <v>471175.02426099998</v>
+      </c>
+      <c r="I16" s="4">
+        <f t="shared" si="0"/>
+        <v>156.47999999999999</v>
+      </c>
+      <c r="J16" s="4">
+        <f t="shared" si="1"/>
+        <v>479913.17133600003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -2202,8 +2472,20 @@
       <c r="F18" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="3">
         <v>20</v>
       </c>
@@ -2222,8 +2504,22 @@
       <c r="F19" s="2">
         <v>439995.98181799997</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19" s="2">
+        <v>21</v>
+      </c>
+      <c r="H19" s="2">
+        <v>468909.38285699999</v>
+      </c>
+      <c r="I19" s="5">
+        <f t="shared" ref="I19:I33" si="2">AVERAGE(C19,D19,G19)</f>
+        <v>19.64</v>
+      </c>
+      <c r="J19" s="5">
+        <f t="shared" ref="J19:J33" si="3">AVERAGE(E19,F19,H19)</f>
+        <v>459241.87652533333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="B20">
         <v>8</v>
       </c>
@@ -2239,8 +2535,22 @@
       <c r="F20">
         <v>478329.28666699998</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20">
+        <v>36.36</v>
+      </c>
+      <c r="H20">
+        <v>457484.43234300002</v>
+      </c>
+      <c r="I20" s="4">
+        <f t="shared" si="2"/>
+        <v>36.36</v>
+      </c>
+      <c r="J20" s="4">
+        <f t="shared" si="3"/>
+        <v>479207.68738233339</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="B21">
         <v>12</v>
       </c>
@@ -2256,8 +2566,22 @@
       <c r="F21">
         <v>489184.26059299998</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21">
+        <v>55.2</v>
+      </c>
+      <c r="H21">
+        <v>478488.971739</v>
+      </c>
+      <c r="I21" s="4">
+        <f t="shared" si="2"/>
+        <v>57.319999999999993</v>
+      </c>
+      <c r="J21" s="4">
+        <f t="shared" si="3"/>
+        <v>484477.26307266665</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="B22">
         <v>16</v>
       </c>
@@ -2273,8 +2597,22 @@
       <c r="F22">
         <v>489729.496835</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22">
+        <v>71.040000000000006</v>
+      </c>
+      <c r="H22">
+        <v>492779.67567600001</v>
+      </c>
+      <c r="I22" s="4">
+        <f t="shared" si="2"/>
+        <v>74</v>
+      </c>
+      <c r="J22" s="4">
+        <f t="shared" si="3"/>
+        <v>490616.68742899998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="B23">
         <v>20</v>
       </c>
@@ -2290,8 +2628,22 @@
       <c r="F23">
         <v>481546.51935900003</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23">
+        <v>89.64</v>
+      </c>
+      <c r="H23">
+        <v>495759.746988</v>
+      </c>
+      <c r="I23" s="4">
+        <f t="shared" si="2"/>
+        <v>89.56</v>
+      </c>
+      <c r="J23" s="4">
+        <f t="shared" si="3"/>
+        <v>491929.24984099995</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="3">
         <v>30</v>
       </c>
@@ -2310,8 +2662,22 @@
       <c r="F24" s="2">
         <v>467119.860759</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24" s="2">
+        <v>29.28</v>
+      </c>
+      <c r="H24" s="2">
+        <v>454190.32786899997</v>
+      </c>
+      <c r="I24" s="5">
+        <f t="shared" si="2"/>
+        <v>28.560000000000002</v>
+      </c>
+      <c r="J24" s="5">
+        <f t="shared" si="3"/>
+        <v>455371.74384866661</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="B25">
         <v>8</v>
       </c>
@@ -2327,8 +2693,22 @@
       <c r="F25">
         <v>476871.41333299997</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25">
+        <v>59.4</v>
+      </c>
+      <c r="H25">
+        <v>482279.41616199998</v>
+      </c>
+      <c r="I25" s="4">
+        <f t="shared" si="2"/>
+        <v>56.199999999999996</v>
+      </c>
+      <c r="J25" s="4">
+        <f t="shared" si="3"/>
+        <v>482930.41345499997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="B26">
         <v>12</v>
       </c>
@@ -2344,8 +2724,22 @@
       <c r="F26">
         <v>476127.41617600003</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26">
+        <v>81.599999999999994</v>
+      </c>
+      <c r="H26">
+        <v>496432.17647100001</v>
+      </c>
+      <c r="I26" s="4">
+        <f t="shared" si="2"/>
+        <v>81.44</v>
+      </c>
+      <c r="J26" s="4">
+        <f t="shared" si="3"/>
+        <v>487542.9302906667</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="B27">
         <v>16</v>
       </c>
@@ -2361,8 +2755,22 @@
       <c r="F27">
         <v>495736.86140699999</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27">
+        <v>111</v>
+      </c>
+      <c r="H27">
+        <v>496507.15243199997</v>
+      </c>
+      <c r="I27" s="4">
+        <f t="shared" si="2"/>
+        <v>111.48</v>
+      </c>
+      <c r="J27" s="4">
+        <f t="shared" si="3"/>
+        <v>493282.007499</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="B28">
         <v>20</v>
       </c>
@@ -2378,8 +2786,22 @@
       <c r="F28">
         <v>488990.25719400001</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28">
+        <v>136.44</v>
+      </c>
+      <c r="H28">
+        <v>501301.65259499999</v>
+      </c>
+      <c r="I28" s="4">
+        <f t="shared" si="2"/>
+        <v>136</v>
+      </c>
+      <c r="J28" s="4">
+        <f t="shared" si="3"/>
+        <v>499561.83613299998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="3">
         <v>40</v>
       </c>
@@ -2398,8 +2820,22 @@
       <c r="F29" s="2">
         <v>465654.49116600002</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29" s="2">
+        <v>39</v>
+      </c>
+      <c r="H29" s="2">
+        <v>451078.969231</v>
+      </c>
+      <c r="I29" s="5">
+        <f t="shared" si="2"/>
+        <v>37.56</v>
+      </c>
+      <c r="J29" s="5">
+        <f t="shared" si="3"/>
+        <v>460283.83120999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="B30">
         <v>8</v>
       </c>
@@ -2415,8 +2851,22 @@
       <c r="F30">
         <v>477918.27113200002</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30">
+        <v>75</v>
+      </c>
+      <c r="H30">
+        <v>486912.93440000003</v>
+      </c>
+      <c r="I30" s="4">
+        <f t="shared" si="2"/>
+        <v>74.52</v>
+      </c>
+      <c r="J30" s="4">
+        <f t="shared" si="3"/>
+        <v>480831.76518266666</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="B31">
         <v>12</v>
       </c>
@@ -2432,8 +2882,22 @@
       <c r="F31">
         <v>486030.79936300003</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31">
+        <v>112.68</v>
+      </c>
+      <c r="H31">
+        <v>487157.72524</v>
+      </c>
+      <c r="I31" s="4">
+        <f t="shared" si="2"/>
+        <v>112.2</v>
+      </c>
+      <c r="J31" s="4">
+        <f t="shared" si="3"/>
+        <v>490162.188937</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="B32">
         <v>16</v>
       </c>
@@ -2449,8 +2913,22 @@
       <c r="F32">
         <v>482466.15189899999</v>
       </c>
-    </row>
-    <row r="33" spans="2:6">
+      <c r="G32">
+        <v>144.84</v>
+      </c>
+      <c r="H32">
+        <v>495454.62303199997</v>
+      </c>
+      <c r="I32" s="4">
+        <f t="shared" si="2"/>
+        <v>142.88</v>
+      </c>
+      <c r="J32" s="4">
+        <f t="shared" si="3"/>
+        <v>491219.78316899994</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10">
       <c r="B33">
         <v>20</v>
       </c>
@@ -2465,6 +2943,20 @@
       </c>
       <c r="F33">
         <v>501971.86983500002</v>
+      </c>
+      <c r="G33">
+        <v>177.36</v>
+      </c>
+      <c r="H33">
+        <v>499167.46887699998</v>
+      </c>
+      <c r="I33" s="4">
+        <f t="shared" si="2"/>
+        <v>173.92</v>
+      </c>
+      <c r="J33" s="4">
+        <f t="shared" si="3"/>
+        <v>498669.63218000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>